<commit_message>
Added support for registering inputs as type 'Q'
</commit_message>
<xml_diff>
--- a/Tests/tests.xlsx
+++ b/Tests/tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waite\Documents\GitHub\tbXLLerator\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4204EC-F226-4E4B-84ED-D50E18BBC38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7BE7BE-5ECD-46AA-B5DE-326D8600143D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1464" yWindow="396" windowWidth="16818" windowHeight="13284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="testNamedRange" localSheetId="0">'udf tests'!$C$32</definedName>
+    <definedName name="testNamedRange" localSheetId="0">'udf tests'!$C$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -546,11 +546,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -592,7 +592,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="str">
-        <f t="shared" ref="A3:A19" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
+        <f t="shared" ref="A3:A22" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
         <v>=TBXLL_Multiply("10","2")</v>
       </c>
       <c r="B3" s="3" cm="1">
@@ -635,71 +635,71 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_AddOptional(1,2)</v>
+        <v>=TBXLL_MultiplyQ(10,2)</v>
       </c>
       <c r="B6" s="3" cm="1">
-        <f t="array" ref="B6">_xll.TBXLL_AddOptional(1,2)</f>
-        <v>3</v>
+        <f t="array" ref="B6">_xll.TBXLL_MultiplyQ(10,2)</f>
+        <v>20</v>
       </c>
       <c r="C6" s="6"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="str">
+        <f t="shared" ref="A7:A8" ca="1" si="1">_xlfn.FORMULATEXT(B7)</f>
+        <v>=TBXLL_MultiplyQ(D4,E4)</v>
+      </c>
+      <c r="B7" s="3" cm="1">
+        <f t="array" ref="B7">_xll.TBXLL_MultiplyQ(D4,E4)</f>
+        <v>20</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=TBXLL_MultiplyQ(Sheet2!D5,Sheet2!E5)</v>
+      </c>
+      <c r="B8" s="3" cm="1">
+        <f t="array" ref="B8">_xll.TBXLL_MultiplyQ(Sheet2!D5,Sheet2!E5)</f>
+        <v>20</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=TBXLL_AddOptional(1,2)</v>
+      </c>
+      <c r="B9" s="3" cm="1">
+        <f t="array" ref="B9">_xll.TBXLL_AddOptional(1,2)</f>
+        <v>3</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>=TBXLL_AddOptional(1,2,3)</v>
       </c>
-      <c r="B7" s="3" cm="1">
-        <f t="array" ref="B7">_xll.TBXLL_AddOptional(1,2,3)</f>
+      <c r="B10" s="3" cm="1">
+        <f t="array" ref="B10">_xll.TBXLL_AddOptional(1,2,3)</f>
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="3" t="str">
+      <c r="C10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>=TBXLL_AlwaysDiv0()</v>
       </c>
-      <c r="B8" s="3" t="e" cm="1">
-        <f t="array" ref="B8">_xll.TBXLL_AlwaysDiv0()</f>
+      <c r="B11" s="3" t="e" cm="1">
+        <f t="array" ref="B11">_xll.TBXLL_AlwaysDiv0()</f>
         <v>#DIV/0!</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B9)</f>
-        <v>=TBXLL_Divide(10,0)</v>
-      </c>
-      <c r="B9" s="3" t="e" cm="1">
-        <f t="array" ref="B9">_xll.TBXLL_Divide(10,0)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B10)</f>
-        <v>=TBXLL_FailAfterSum({1,2,3})</v>
-      </c>
-      <c r="B10" s="3" t="e" cm="1">
-        <f t="array" ref="B10">_xll.TBXLL_FailAfterSum({1,2,3})</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B11)</f>
-        <v>=TBXLL_NotFound()</v>
-      </c>
-      <c r="B11" s="3" t="e" cm="1">
-        <f t="array" ref="B11">_xll.TBXLL_NotFound()</f>
-        <v>#N/A</v>
       </c>
       <c r="C11" s="6"/>
       <c r="H11" s="7"/>
@@ -707,11 +707,11 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B12)</f>
-        <v>=TBXLL_SqrtChecked(-1)</v>
+        <v>=TBXLL_Divide(10,0)</v>
       </c>
       <c r="B12" s="3" t="e" cm="1">
-        <f t="array" ref="B12">_xll.TBXLL_SqrtChecked(-1)</f>
-        <v>#NUM!</v>
+        <f t="array" ref="B12">_xll.TBXLL_Divide(10,0)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="C12" s="6"/>
       <c r="H12" s="7"/>
@@ -719,10 +719,10 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B13)</f>
-        <v>=TBXLL_TextOnly(25)</v>
+        <v>=TBXLL_FailAfterSum({1,2,3})</v>
       </c>
       <c r="B13" s="3" t="e" cm="1">
-        <f t="array" ref="B13">_xll.TBXLL_TextOnly(25)</f>
+        <f t="array" ref="B13">_xll.TBXLL_FailAfterSum({1,2,3})</f>
         <v>#VALUE!</v>
       </c>
       <c r="C13" s="6"/>
@@ -730,522 +730,558 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_Average({1,2,3})</v>
-      </c>
-      <c r="B14" s="3" cm="1">
-        <f t="array" ref="B14">_xll.TBXLL_Average({1,2,3})</f>
-        <v>2</v>
+        <f ca="1">_xlfn.FORMULATEXT(B14)</f>
+        <v>=TBXLL_NotFound()</v>
+      </c>
+      <c r="B14" s="3" t="e" cm="1">
+        <f t="array" ref="B14">_xll.TBXLL_NotFound()</f>
+        <v>#N/A</v>
       </c>
       <c r="C14" s="6"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_ConditionalAdd(10,D15,"result")</v>
-      </c>
-      <c r="B15" s="3" t="str" cm="1">
-        <f t="array" ref="B15">_xll.TBXLL_ConditionalAdd(10,D15,"result")</f>
-        <v>result: 20</v>
+        <f ca="1">_xlfn.FORMULATEXT(B15)</f>
+        <v>=TBXLL_SqrtChecked(-1)</v>
+      </c>
+      <c r="B15" s="3" t="e" cm="1">
+        <f t="array" ref="B15">_xll.TBXLL_SqrtChecked(-1)</f>
+        <v>#NUM!</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_ConditionalAdd(10,D16,"result")</v>
-      </c>
-      <c r="B16" s="3" t="str" cm="1">
-        <f t="array" ref="B16">_xll.TBXLL_ConditionalAdd(10,D16,"result")</f>
-        <v>result: 10</v>
+        <f ca="1">_xlfn.FORMULATEXT(B16)</f>
+        <v>=TBXLL_TextOnly(25)</v>
+      </c>
+      <c r="B16" s="3" t="e" cm="1">
+        <f t="array" ref="B16">_xll.TBXLL_TextOnly(25)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C16" s="6"/>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_CountIf(D17:F17,"&gt;=3")</v>
+        <v>=TBXLL_Average({1,2,3})</v>
       </c>
       <c r="B17" s="3" cm="1">
-        <f t="array" ref="B17">_xll.TBXLL_CountIf(D17:F17,"&gt;=3")</f>
+        <f t="array" ref="B17">_xll.TBXLL_Average({1,2,3})</f>
         <v>2</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="F17">
-        <v>4</v>
-      </c>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_Now()</v>
-      </c>
-      <c r="B18" s="4" cm="1">
-        <f t="array" aca="1" ref="B18" ca="1">_xll.TBXLL_Now()</f>
-        <v>46080.28896377315</v>
-      </c>
-      <c r="C18" s="12"/>
+        <v>=TBXLL_ConditionalAdd(10,D18,"result")</v>
+      </c>
+      <c r="B18" s="3" t="str" cm="1">
+        <f t="array" ref="B18">_xll.TBXLL_ConditionalAdd(10,D18,"result")</f>
+        <v>result: 20</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
       <c r="H18" s="7"/>
-      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=NOW()</v>
-      </c>
-      <c r="B19" s="4">
-        <f ca="1">NOW()</f>
-        <v>46080.28896377315</v>
+        <v>=TBXLL_ConditionalAdd(10,D19,"result")</v>
+      </c>
+      <c r="B19" s="3" t="str" cm="1">
+        <f t="array" ref="B19">_xll.TBXLL_ConditionalAdd(10,D19,"result")</f>
+        <v>result: 10</v>
       </c>
       <c r="C19" s="6"/>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B20)</f>
-        <v>=TBXLL_SqrtChecked(9)</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>=TBXLL_CountIf(D20:F20,"&gt;=3")</v>
       </c>
       <c r="B20" s="3" cm="1">
-        <f t="array" ref="B20">_xll.TBXLL_SqrtChecked(9)</f>
+        <f t="array" ref="B20">_xll.TBXLL_CountIf(D20:F20,"&gt;=3")</f>
+        <v>2</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
         <v>3</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="F20">
+        <v>4</v>
+      </c>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B21)</f>
-        <v>=TBXLL_TextOnly("25")</v>
-      </c>
-      <c r="B21" s="3" t="str" cm="1">
-        <f t="array" ref="B21">_xll.TBXLL_TextOnly("25")</f>
-        <v>OK: 25</v>
-      </c>
-      <c r="C21" s="6"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>=TBXLL_Now()</v>
+      </c>
+      <c r="B21" s="4" cm="1">
+        <f t="array" aca="1" ref="B21" ca="1">_xll.TBXLL_Now()</f>
+        <v>46080.42014884259</v>
+      </c>
+      <c r="C21" s="12"/>
       <c r="H21" s="7"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B22)</f>
-        <v>=TBXLL_Transpose({1;2;3})</v>
-      </c>
-      <c r="B22" s="3" cm="1">
-        <f t="array" ref="B22:D22">_xll.TBXLL_Transpose({1;2;3})</f>
-        <v>1</v>
-      </c>
-      <c r="C22" s="6">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
+        <f t="shared" ca="1" si="0"/>
+        <v>=NOW()</v>
+      </c>
+      <c r="B22" s="4">
+        <f ca="1">NOW()</f>
+        <v>46080.42014884259</v>
+      </c>
+      <c r="C22" s="6"/>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="str">
-        <f t="shared" ref="A23:A31" ca="1" si="1">_xlfn.FORMULATEXT(B23)</f>
-        <v>=TBXLL_Upper("mike")</v>
-      </c>
-      <c r="B23" s="3" t="str" cm="1">
-        <f t="array" ref="B23">_xll.TBXLL_Upper("mike")</f>
-        <v>MIKE</v>
+        <f ca="1">_xlfn.FORMULATEXT(B23)</f>
+        <v>=TBXLL_SqrtChecked(9)</v>
+      </c>
+      <c r="B23" s="3" cm="1">
+        <f t="array" ref="B23">_xll.TBXLL_SqrtChecked(9)</f>
+        <v>3</v>
       </c>
       <c r="C23" s="6"/>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=TBXLL_RecalcCounter()</v>
-      </c>
-      <c r="B24" s="3" cm="1">
-        <f t="array" aca="1" ref="B24" ca="1">_xll.TBXLL_RecalcCounter()</f>
-        <v>2</v>
+        <f ca="1">_xlfn.FORMULATEXT(B24)</f>
+        <v>=TBXLL_TextOnly("25")</v>
+      </c>
+      <c r="B24" s="3" t="str" cm="1">
+        <f t="array" ref="B24">_xll.TBXLL_TextOnly("25")</f>
+        <v>OK: 25</v>
       </c>
       <c r="C24" s="6"/>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=TBXLL_SumArray({1,2,3})</v>
+        <f ca="1">_xlfn.FORMULATEXT(B25)</f>
+        <v>=TBXLL_Transpose({1;2;3})</v>
       </c>
       <c r="B25" s="3" cm="1">
-        <f t="array" ref="B25">_xll.TBXLL_SumArray({1,2,3})</f>
-        <v>6</v>
-      </c>
-      <c r="C25" s="6"/>
+        <f t="array" ref="B25:D25">_xll.TBXLL_Transpose({1;2;3})</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=TBXLL_SumArray2({1,2,3})</v>
-      </c>
-      <c r="B26" s="3" cm="1">
-        <f t="array" ref="B26">_xll.TBXLL_SumArray2({1,2,3})</f>
-        <v>6</v>
+        <f t="shared" ref="A26:A34" ca="1" si="2">_xlfn.FORMULATEXT(B26)</f>
+        <v>=TBXLL_Upper("mike")</v>
+      </c>
+      <c r="B26" s="3" t="str" cm="1">
+        <f t="array" ref="B26">_xll.TBXLL_Upper("mike")</f>
+        <v>MIKE</v>
       </c>
       <c r="C26" s="6"/>
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>{=TBXLL_Join(D27:F28,TRUE)}</v>
-      </c>
-      <c r="B27" s="3" t="str">
-        <f t="array" ref="B27">_xll.TBXLL_Join(D27:F28,TRUE)</f>
-        <v>rc11,rc21,rc12,rc22,rc13,rc23</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_RecalcCounter()</v>
+      </c>
+      <c r="B27" s="3" cm="1">
+        <f t="array" aca="1" ref="B27" ca="1">_xll.TBXLL_RecalcCounter()</f>
+        <v>9</v>
       </c>
       <c r="C27" s="6"/>
-      <c r="D27" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>2</v>
-      </c>
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=TBXLL_Join(D27:F28,FALSE)</v>
-      </c>
-      <c r="B28" s="3" t="str" cm="1">
-        <f t="array" ref="B28">_xll.TBXLL_Join(D27:F28,FALSE)</f>
-        <v>rc11,rc12,rc13,rc21,rc22,rc23</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_SumArray({1,2,3})</v>
+      </c>
+      <c r="B28" s="3" cm="1">
+        <f t="array" ref="B28">_xll.TBXLL_SumArray({1,2,3})</f>
+        <v>6</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" t="s">
-        <v>5</v>
-      </c>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=TBXLL_Join({11,12,13;21,22,23},TRUE)</v>
-      </c>
-      <c r="B29" s="3" t="str" cm="1">
-        <f t="array" ref="B29">_xll.TBXLL_Join({11,12,13;21,22,23},TRUE)</f>
-        <v>11,21,12,22,13,23</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_SumArray2({1,2,3})</v>
+      </c>
+      <c r="B29" s="3" cm="1">
+        <f t="array" ref="B29">_xll.TBXLL_SumArray2({1,2,3})</f>
+        <v>6</v>
       </c>
       <c r="C29" s="6"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=TBXLL_Join({11,12,13;21,22,23},FALSE)</v>
-      </c>
-      <c r="B30" s="3" t="str" cm="1">
-        <f t="array" ref="B30">_xll.TBXLL_Join({11,12,13;21,22,23},FALSE)</f>
-        <v>11,12,13,21,22,23</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>{=TBXLL_Join(D30:F31,TRUE)}</v>
+      </c>
+      <c r="B30" s="3" t="str">
+        <f t="array" ref="B30">_xll.TBXLL_Join(D30:F31,TRUE)</f>
+        <v>rc11,rc21,rc12,rc22,rc13,rc23</v>
       </c>
       <c r="C30" s="6"/>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>=TBXLL_Join({11,12,13;21,22,23})</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_Join(D30:F31,FALSE)</v>
       </c>
       <c r="B31" s="3" t="str" cm="1">
-        <f t="array" ref="B31">_xll.TBXLL_Join({11,12,13;21,22,23})</f>
-        <v>11,12,13,21,22,23</v>
+        <f t="array" ref="B31">_xll.TBXLL_Join(D30:F31,FALSE)</f>
+        <v>rc11,rc12,rc13,rc21,rc22,rc23</v>
       </c>
       <c r="C31" s="6"/>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="str">
-        <f t="shared" ref="A32:A42" ca="1" si="2">_xlfn.FORMULATEXT(B32)</f>
-        <v>=TBXLL_CellValue(testNamedRange)</v>
-      </c>
-      <c r="B32" s="3" t="b" cm="1">
-        <f t="array" ref="B32">_xll.TBXLL_CellValue(testNamedRange)</f>
-        <v>1</v>
-      </c>
-      <c r="C32" s="6" t="b">
-        <v>1</v>
-      </c>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_Join({11,12,13;21,22,23},TRUE)</v>
+      </c>
+      <c r="B32" s="3" t="str" cm="1">
+        <f t="array" ref="B32">_xll.TBXLL_Join({11,12,13;21,22,23},TRUE)</f>
+        <v>11,21,12,22,13,23</v>
+      </c>
+      <c r="C32" s="6"/>
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_CellValue(C33)</v>
-      </c>
-      <c r="B33" s="3" cm="1">
-        <f t="array" ref="B33">_xll.TBXLL_CellValue(C33)</f>
-        <v>99</v>
-      </c>
-      <c r="C33" s="6">
-        <v>99</v>
-      </c>
+        <v>=TBXLL_Join({11,12,13;21,22,23},FALSE)</v>
+      </c>
+      <c r="B33" s="3" t="str" cm="1">
+        <f t="array" ref="B33">_xll.TBXLL_Join({11,12,13;21,22,23},FALSE)</f>
+        <v>11,12,13,21,22,23</v>
+      </c>
+      <c r="C33" s="6"/>
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_SheetName(D34)</v>
+        <v>=TBXLL_Join({11,12,13;21,22,23})</v>
       </c>
       <c r="B34" s="3" t="str" cm="1">
-        <f t="array" ref="B34">_xll.TBXLL_SheetName(D34)</f>
-        <v>[tests.xlsx]udf tests</v>
+        <f t="array" ref="B34">_xll.TBXLL_Join({11,12,13;21,22,23})</f>
+        <v>11,12,13,21,22,23</v>
       </c>
       <c r="C34" s="6"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B35)</f>
-        <v>=TBXLL_CellAddress(C35)</v>
-      </c>
-      <c r="B35" s="13" t="str" cm="1">
-        <f t="array" ref="B35">_xll.TBXLL_CellAddress(C35)</f>
-        <v>$C$35</v>
-      </c>
-      <c r="C35" s="6"/>
+        <f t="shared" ref="A35:A45" ca="1" si="3">_xlfn.FORMULATEXT(B35)</f>
+        <v>=TBXLL_CellValue(testNamedRange)</v>
+      </c>
+      <c r="B35" s="3" t="b" cm="1">
+        <f t="array" ref="B35">_xll.TBXLL_CellValue(testNamedRange)</f>
+        <v>1</v>
+      </c>
+      <c r="C35" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B36)</f>
-        <v>=TBXLL_CellAddress(Sheet2!C35)</v>
-      </c>
-      <c r="B36" s="13" t="str" cm="1">
-        <f t="array" ref="B36">_xll.TBXLL_CellAddress(Sheet2!C35)</f>
-        <v>$C$35</v>
-      </c>
-      <c r="C36" s="6"/>
+        <f t="shared" ca="1" si="3"/>
+        <v>=TBXLL_CellValue(C36)</v>
+      </c>
+      <c r="B36" s="3" cm="1">
+        <f t="array" ref="B36">_xll.TBXLL_CellValue(C36)</f>
+        <v>99</v>
+      </c>
+      <c r="C36" s="6">
+        <v>99</v>
+      </c>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B37)</f>
-        <v>=TBXLL_CellAddress_Hidden(C35)</v>
-      </c>
-      <c r="B37" s="13" t="str" cm="1">
-        <f t="array" ref="B37">_xll.TBXLL_CellAddress_Hidden(C35)</f>
-        <v>$C$35</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=TBXLL_SheetName(D37)</v>
+      </c>
+      <c r="B37" s="3" t="str" cm="1">
+        <f t="array" ref="B37">_xll.TBXLL_SheetName(D37)</f>
+        <v>[tests.xlsx]udf tests</v>
       </c>
       <c r="C37" s="6"/>
-      <c r="D37" s="13"/>
       <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_IsEmptyCell(C38)</v>
-      </c>
-      <c r="B38" s="3" t="b" cm="1">
-        <f t="array" ref="B38">_xll.TBXLL_IsEmptyCell(C38)</f>
-        <v>1</v>
+        <f ca="1">_xlfn.FORMULATEXT(B38)</f>
+        <v>=TBXLL_CellAddress(C38)</v>
+      </c>
+      <c r="B38" s="13" t="str" cm="1">
+        <f t="array" ref="B38">_xll.TBXLL_CellAddress(C38)</f>
+        <v>$C$38</v>
       </c>
       <c r="C38" s="6"/>
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_TestMissing(3.6)</v>
-      </c>
-      <c r="B39" s="3" cm="1">
-        <f t="array" ref="B39">_xll.TBXLL_TestMissing(3.6)</f>
-        <v>4</v>
+        <f ca="1">_xlfn.FORMULATEXT(B39)</f>
+        <v>=TBXLL_CellAddress(Sheet2!C35)</v>
+      </c>
+      <c r="B39" s="13" t="str" cm="1">
+        <f t="array" ref="B39">_xll.TBXLL_CellAddress(Sheet2!C35)</f>
+        <v>$C$35</v>
       </c>
       <c r="C39" s="6"/>
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>{=TBXLL_MultiplyArrays(D40:D42,E40:E42)}</v>
-      </c>
-      <c r="B40" s="3">
-        <f t="array" ref="B40:B42">_xll.TBXLL_MultiplyArrays(D40:D42,E40:E42)</f>
-        <v>2</v>
+        <f ca="1">_xlfn.FORMULATEXT(B40)</f>
+        <v>=TBXLL_CellAddress_Hidden(C38)</v>
+      </c>
+      <c r="B40" s="13" t="str" cm="1">
+        <f t="array" ref="B40">_xll.TBXLL_CellAddress_Hidden(C38)</f>
+        <v>$C$38</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
+      <c r="D40" s="13"/>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>{=TBXLL_MultiplyArrays(D40:D42,E40:E42)}</v>
-      </c>
-      <c r="B41" s="3">
-        <v>20</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=TBXLL_IsEmptyCell(C41)</v>
+      </c>
+      <c r="B41" s="3" t="b" cm="1">
+        <f t="array" ref="B41">_xll.TBXLL_IsEmptyCell(C41)</f>
+        <v>1</v>
       </c>
       <c r="C41" s="6"/>
-      <c r="D41">
-        <v>4</v>
-      </c>
-      <c r="E41">
-        <v>5</v>
-      </c>
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>{=TBXLL_MultiplyArrays(D40:D42,E40:E42)}</v>
-      </c>
-      <c r="B42" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>=TBXLL_TestMissing(3.6)</v>
+      </c>
+      <c r="B42" s="3" cm="1">
+        <f t="array" ref="B42">_xll.TBXLL_TestMissing(3.6)</f>
         <v>4</v>
       </c>
       <c r="C42" s="6"/>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="str">
-        <f t="shared" ref="A43:A50" ca="1" si="3">_xlfn.FORMULATEXT(B43)</f>
-        <v>{=TBXLL_NormalizeArray({4,9,16,25})}</v>
-      </c>
-      <c r="B43" s="5">
-        <f t="array" ref="B43:E43">_xll.TBXLL_NormalizeArray({4,9,16,25})</f>
-        <v>7.407407407407407E-2</v>
-      </c>
-      <c r="C43" s="8">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D43" s="9">
-        <v>0.29629629629629628</v>
-      </c>
-      <c r="E43" s="9">
-        <v>0.46296296296296297</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>{=TBXLL_MultiplyArrays(D43:D45,E43:E45)}</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="array" ref="B43:B45">_xll.TBXLL_MultiplyArrays(D43:D45,E43:E45)</f>
+        <v>2</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
       </c>
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_SpeedSafe(100)</v>
-      </c>
-      <c r="B44" s="3" cm="1">
-        <f t="array" ref="B44">_xll.TBXLL_SpeedSafe(100)</f>
-        <v>66671645.919710793</v>
+        <v>{=TBXLL_MultiplyArrays(D43:D45,E43:E45)}</v>
+      </c>
+      <c r="B44" s="3">
+        <v>20</v>
       </c>
       <c r="C44" s="6"/>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_SpeedUnsafe(100)</v>
-      </c>
-      <c r="B45" s="3" cm="1">
-        <f t="array" ref="B45">_xll.TBXLL_SpeedUnsafe(100)</f>
-        <v>66671645.919710793</v>
+        <v>{=TBXLL_MultiplyArrays(D43:D45,E43:E45)}</v>
+      </c>
+      <c r="B45" s="3">
+        <v>4</v>
       </c>
       <c r="C45" s="6"/>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="str">
-        <f t="shared" ref="A46" ca="1" si="4">_xlfn.FORMULATEXT(B46)</f>
-        <v>=TBXLL_Timestamp()</v>
-      </c>
-      <c r="B46" s="16" cm="1">
-        <f t="array" aca="1" ref="B46" ca="1">_xll.TBXLL_Timestamp()</f>
-        <v>153756.47553669999</v>
-      </c>
-      <c r="C46" s="6"/>
+        <f t="shared" ref="A46:A53" ca="1" si="4">_xlfn.FORMULATEXT(B46)</f>
+        <v>{=TBXLL_NormalizeArray({4,9,16,25})}</v>
+      </c>
+      <c r="B46" s="5">
+        <f t="array" ref="B46:E46">_xll.TBXLL_NormalizeArray({4,9,16,25})</f>
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="C46" s="8">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="E46" s="9">
+        <v>0.46296296296296297</v>
+      </c>
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_NumberName(9)</v>
-      </c>
-      <c r="B47" s="3" t="str" cm="1">
-        <f t="array" ref="B47">_xll.TBXLL_NumberName(9)</f>
-        <v>Nine</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_SpeedSafe(100)</v>
+      </c>
+      <c r="B47" s="3" cm="1">
+        <f t="array" ref="B47">_xll.TBXLL_SpeedSafe(100)</f>
+        <v>66671645.919710793</v>
       </c>
       <c r="C47" s="6"/>
       <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_RomanNumeral(9)</v>
-      </c>
-      <c r="B48" s="3" t="str" cm="1">
-        <f t="array" ref="B48">_xll.TBXLL_RomanNumeral(9)</f>
-        <v>IX</v>
-      </c>
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_SpeedUnsafe(100)</v>
+      </c>
+      <c r="B48" s="3" cm="1">
+        <f t="array" ref="B48">_xll.TBXLL_SpeedUnsafe(100)</f>
+        <v>66671645.919710793</v>
+      </c>
+      <c r="C48" s="6"/>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_AddDays(NOW(),7)</v>
-      </c>
-      <c r="B49" s="14" cm="1">
-        <f t="array" aca="1" ref="B49" ca="1">_xll.TBXLL_AddDays(NOW(),7)</f>
-        <v>46087.28896377315</v>
+        <f t="shared" ref="A49" ca="1" si="5">_xlfn.FORMULATEXT(B49)</f>
+        <v>=TBXLL_Timestamp()</v>
+      </c>
+      <c r="B49" s="16" cm="1">
+        <f t="array" aca="1" ref="B49" ca="1">_xll.TBXLL_Timestamp()</f>
+        <v>165090.87213120001</v>
       </c>
       <c r="C49" s="6"/>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_NumberName(9)</v>
+      </c>
+      <c r="B50" s="3" t="str" cm="1">
+        <f t="array" ref="B50">_xll.TBXLL_NumberName(9)</f>
+        <v>Nine</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_RomanNumeral(9)</v>
+      </c>
+      <c r="B51" s="3" t="str" cm="1">
+        <f t="array" ref="B51">_xll.TBXLL_RomanNumeral(9)</f>
+        <v>IX</v>
+      </c>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_AddDays(NOW(),7)</v>
+      </c>
+      <c r="B52" s="14" cm="1">
+        <f t="array" aca="1" ref="B52" ca="1">_xll.TBXLL_AddDays(NOW(),7)</f>
+        <v>46087.42014884259</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
         <v>=TBXLL_FormatArray({1,2,3},"item")</v>
       </c>
-      <c r="B50" s="13" t="str" cm="1">
-        <f t="array" ref="B50:D50">_xll.TBXLL_FormatArray({1,2,3},"item")</f>
+      <c r="B53" s="13" t="str" cm="1">
+        <f t="array" ref="B53:D53">_xll.TBXLL_FormatArray({1,2,3},"item")</f>
         <v>item_1</v>
       </c>
-      <c r="C50" s="15" t="str">
+      <c r="C53" s="15" t="str">
         <v>item_2</v>
       </c>
-      <c r="D50" s="10" t="str">
+      <c r="D53" s="10" t="str">
         <v>item_3</v>
       </c>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="11"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Renamed Bind to BindU
</commit_message>
<xml_diff>
--- a/Tests/tests.xlsx
+++ b/Tests/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waite\Documents\GitHub\tbXLLerator\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7BE7BE-5ECD-46AA-B5DE-326D8600143D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B2132F-DB37-4FBF-869D-265E11159995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="396" windowWidth="16818" windowHeight="13284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="396" windowWidth="16974" windowHeight="13284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="udf tests" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,6 +265,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -834,7 +835,7 @@
       </c>
       <c r="B21" s="4" cm="1">
         <f t="array" aca="1" ref="B21" ca="1">_xll.TBXLL_Now()</f>
-        <v>46080.42014884259</v>
+        <v>46080.516100578701</v>
       </c>
       <c r="C21" s="12"/>
       <c r="H21" s="7"/>
@@ -847,7 +848,7 @@
       </c>
       <c r="B22" s="4">
         <f ca="1">NOW()</f>
-        <v>46080.42014884259</v>
+        <v>46080.516100578701</v>
       </c>
       <c r="C22" s="6"/>
       <c r="H22" s="7"/>
@@ -912,7 +913,7 @@
       </c>
       <c r="B27" s="3" cm="1">
         <f t="array" aca="1" ref="B27" ca="1">_xll.TBXLL_RecalcCounter()</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C27" s="6"/>
       <c r="H27" s="7"/>
@@ -1093,7 +1094,7 @@
         <v>$C$38</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="13"/>
+      <c r="D40" s="20"/>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1223,7 +1224,7 @@
       </c>
       <c r="B49" s="16" cm="1">
         <f t="array" aca="1" ref="B49" ca="1">_xll.TBXLL_Timestamp()</f>
-        <v>165090.87213120001</v>
+        <v>173381.10888690001</v>
       </c>
       <c r="C49" s="6"/>
       <c r="H49" s="7"/>
@@ -1258,7 +1259,7 @@
       </c>
       <c r="B52" s="14" cm="1">
         <f t="array" aca="1" ref="B52" ca="1">_xll.TBXLL_AddDays(NOW(),7)</f>
-        <v>46087.42014884259</v>
+        <v>46087.516100578701</v>
       </c>
       <c r="C52" s="6"/>
       <c r="H52" s="7"/>

</xml_diff>

<commit_message>
Renamed Reg Data Types
</commit_message>
<xml_diff>
--- a/Tests/tests.xlsx
+++ b/Tests/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waite\Documents\GitHub\tbXLLerator\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B2132F-DB37-4FBF-869D-265E11159995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676C0B54-697C-4902-B96A-0E20221193F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="396" windowWidth="16974" windowHeight="13284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4158" yWindow="396" windowWidth="16974" windowHeight="13284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="udf tests" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,7 +265,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +550,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -835,7 +834,7 @@
       </c>
       <c r="B21" s="4" cm="1">
         <f t="array" aca="1" ref="B21" ca="1">_xll.TBXLL_Now()</f>
-        <v>46080.516100578701</v>
+        <v>46081.399229976851</v>
       </c>
       <c r="C21" s="12"/>
       <c r="H21" s="7"/>
@@ -848,7 +847,7 @@
       </c>
       <c r="B22" s="4">
         <f ca="1">NOW()</f>
-        <v>46080.516100578701</v>
+        <v>46081.399229976851</v>
       </c>
       <c r="C22" s="6"/>
       <c r="H22" s="7"/>
@@ -913,7 +912,7 @@
       </c>
       <c r="B27" s="3" cm="1">
         <f t="array" aca="1" ref="B27" ca="1">_xll.TBXLL_RecalcCounter()</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C27" s="6"/>
       <c r="H27" s="7"/>
@@ -1094,7 +1093,6 @@
         <v>$C$38</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="20"/>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1224,7 +1222,7 @@
       </c>
       <c r="B49" s="16" cm="1">
         <f t="array" aca="1" ref="B49" ca="1">_xll.TBXLL_Timestamp()</f>
-        <v>173381.10888690001</v>
+        <v>249685.55196509999</v>
       </c>
       <c r="C49" s="6"/>
       <c r="H49" s="7"/>
@@ -1259,7 +1257,7 @@
       </c>
       <c r="B52" s="14" cm="1">
         <f t="array" aca="1" ref="B52" ca="1">_xll.TBXLL_AddDays(NOW(),7)</f>
-        <v>46087.516100578701</v>
+        <v>46088.399229976851</v>
       </c>
       <c r="C52" s="6"/>
       <c r="H52" s="7"/>

</xml_diff>

<commit_message>
Support and testing for Double (B) and FP12 (K%) argument types
</commit_message>
<xml_diff>
--- a/Tests/tests.xlsx
+++ b/Tests/tests.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waite\Documents\GitHub\tbXLLerator\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676C0B54-697C-4902-B96A-0E20221193F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964C5A80-A916-4AA7-85AA-7E1BAE868523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4158" yWindow="396" windowWidth="16974" windowHeight="13284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="396" windowWidth="19764" windowHeight="13284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="udf tests" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="testNamedRange" localSheetId="0">'udf tests'!$C$35</definedName>
+    <definedName name="testNamedRange" localSheetId="0">'udf tests'!$C$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -125,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -234,11 +234,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -265,6 +287,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,11 +570,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -592,7 +616,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="str">
-        <f t="shared" ref="A3:A22" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
+        <f t="shared" ref="A3:A25" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
         <v>=TBXLL_Multiply("10","2")</v>
       </c>
       <c r="B3" s="3" cm="1">
@@ -646,7 +670,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="str">
-        <f t="shared" ref="A7:A8" ca="1" si="1">_xlfn.FORMULATEXT(B7)</f>
+        <f t="shared" ref="A7:A11" ca="1" si="1">_xlfn.FORMULATEXT(B7)</f>
         <v>=TBXLL_MultiplyQ(D4,E4)</v>
       </c>
       <c r="B7" s="3" cm="1">
@@ -670,72 +694,72 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=TBXLL_MultiplyB(10,2)</v>
+      </c>
+      <c r="B9" s="3" cm="1">
+        <f t="array" ref="B9">_xll.TBXLL_MultiplyB(10,2)</f>
+        <v>20</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=TBXLL_MultiplyB(D4,E4)</v>
+      </c>
+      <c r="B10" s="3" cm="1">
+        <f t="array" ref="B10">_xll.TBXLL_MultiplyB(D4,E4)</f>
+        <v>20</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=TBXLL_MultiplyB(Sheet2!D5,Sheet2!E5)</v>
+      </c>
+      <c r="B11" s="3" cm="1">
+        <f t="array" ref="B11">_xll.TBXLL_MultiplyB(Sheet2!D5,Sheet2!E5)</f>
+        <v>20</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>=TBXLL_AddOptional(1,2)</v>
       </c>
-      <c r="B9" s="3" cm="1">
-        <f t="array" ref="B9">_xll.TBXLL_AddOptional(1,2)</f>
+      <c r="B12" s="3" cm="1">
+        <f t="array" ref="B12">_xll.TBXLL_AddOptional(1,2)</f>
         <v>3</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="3" t="str">
+      <c r="C12" s="6"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>=TBXLL_AddOptional(1,2,3)</v>
       </c>
-      <c r="B10" s="3" cm="1">
-        <f t="array" ref="B10">_xll.TBXLL_AddOptional(1,2,3)</f>
+      <c r="B13" s="3" cm="1">
+        <f t="array" ref="B13">_xll.TBXLL_AddOptional(1,2,3)</f>
         <v>6</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3" t="str">
+      <c r="C13" s="6"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>=TBXLL_AlwaysDiv0()</v>
       </c>
-      <c r="B11" s="3" t="e" cm="1">
-        <f t="array" ref="B11">_xll.TBXLL_AlwaysDiv0()</f>
+      <c r="B14" s="3" t="e" cm="1">
+        <f t="array" ref="B14">_xll.TBXLL_AlwaysDiv0()</f>
         <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B12)</f>
-        <v>=TBXLL_Divide(10,0)</v>
-      </c>
-      <c r="B12" s="3" t="e" cm="1">
-        <f t="array" ref="B12">_xll.TBXLL_Divide(10,0)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B13)</f>
-        <v>=TBXLL_FailAfterSum({1,2,3})</v>
-      </c>
-      <c r="B13" s="3" t="e" cm="1">
-        <f t="array" ref="B13">_xll.TBXLL_FailAfterSum({1,2,3})</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B14)</f>
-        <v>=TBXLL_NotFound()</v>
-      </c>
-      <c r="B14" s="3" t="e" cm="1">
-        <f t="array" ref="B14">_xll.TBXLL_NotFound()</f>
-        <v>#N/A</v>
       </c>
       <c r="C14" s="6"/>
       <c r="H14" s="7"/>
@@ -743,11 +767,11 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B15)</f>
-        <v>=TBXLL_SqrtChecked(-1)</v>
+        <v>=TBXLL_Divide(10,0)</v>
       </c>
       <c r="B15" s="3" t="e" cm="1">
-        <f t="array" ref="B15">_xll.TBXLL_SqrtChecked(-1)</f>
-        <v>#NUM!</v>
+        <f t="array" ref="B15">_xll.TBXLL_Divide(10,0)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="C15" s="6"/>
       <c r="H15" s="7"/>
@@ -755,10 +779,10 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B16)</f>
-        <v>=TBXLL_TextOnly(25)</v>
+        <v>=TBXLL_FailAfterSum({1,2,3})</v>
       </c>
       <c r="B16" s="3" t="e" cm="1">
-        <f t="array" ref="B16">_xll.TBXLL_TextOnly(25)</f>
+        <f t="array" ref="B16">_xll.TBXLL_FailAfterSum({1,2,3})</f>
         <v>#VALUE!</v>
       </c>
       <c r="C16" s="6"/>
@@ -766,177 +790,177 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_Average({1,2,3})</v>
-      </c>
-      <c r="B17" s="3" cm="1">
-        <f t="array" ref="B17">_xll.TBXLL_Average({1,2,3})</f>
-        <v>2</v>
+        <f ca="1">_xlfn.FORMULATEXT(B17)</f>
+        <v>=TBXLL_NotFound()</v>
+      </c>
+      <c r="B17" s="3" t="e" cm="1">
+        <f t="array" ref="B17">_xll.TBXLL_NotFound()</f>
+        <v>#N/A</v>
       </c>
       <c r="C17" s="6"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_ConditionalAdd(10,D18,"result")</v>
-      </c>
-      <c r="B18" s="3" t="str" cm="1">
-        <f t="array" ref="B18">_xll.TBXLL_ConditionalAdd(10,D18,"result")</f>
-        <v>result: 20</v>
+        <f ca="1">_xlfn.FORMULATEXT(B18)</f>
+        <v>=TBXLL_SqrtChecked(-1)</v>
+      </c>
+      <c r="B18" s="3" t="e" cm="1">
+        <f t="array" ref="B18">_xll.TBXLL_SqrtChecked(-1)</f>
+        <v>#NUM!</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_ConditionalAdd(10,D19,"result")</v>
-      </c>
-      <c r="B19" s="3" t="str" cm="1">
-        <f t="array" ref="B19">_xll.TBXLL_ConditionalAdd(10,D19,"result")</f>
-        <v>result: 10</v>
+        <f ca="1">_xlfn.FORMULATEXT(B19)</f>
+        <v>=TBXLL_TextOnly(25)</v>
+      </c>
+      <c r="B19" s="3" t="e" cm="1">
+        <f t="array" ref="B19">_xll.TBXLL_TextOnly(25)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_CountIf(D20:F20,"&gt;=3")</v>
+        <v>=TBXLL_Average({1,2,3})</v>
       </c>
       <c r="B20" s="3" cm="1">
-        <f t="array" ref="B20">_xll.TBXLL_CountIf(D20:F20,"&gt;=3")</f>
+        <f t="array" ref="B20">_xll.TBXLL_Average({1,2,3})</f>
         <v>2</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=TBXLL_Now()</v>
-      </c>
-      <c r="B21" s="4" cm="1">
-        <f t="array" aca="1" ref="B21" ca="1">_xll.TBXLL_Now()</f>
-        <v>46081.399229976851</v>
-      </c>
-      <c r="C21" s="12"/>
+        <v>=TBXLL_ConditionalAdd(10,D21,"result")</v>
+      </c>
+      <c r="B21" s="3" t="str" cm="1">
+        <f t="array" ref="B21">_xll.TBXLL_ConditionalAdd(10,D21,"result")</f>
+        <v>result: 20</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
       <c r="H21" s="7"/>
-      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=NOW()</v>
-      </c>
-      <c r="B22" s="4">
-        <f ca="1">NOW()</f>
-        <v>46081.399229976851</v>
+        <v>=TBXLL_ConditionalAdd(10,D22,"result")</v>
+      </c>
+      <c r="B22" s="3" t="str" cm="1">
+        <f t="array" ref="B22">_xll.TBXLL_ConditionalAdd(10,D22,"result")</f>
+        <v>result: 10</v>
       </c>
       <c r="C22" s="6"/>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B23)</f>
-        <v>=TBXLL_SqrtChecked(9)</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>=TBXLL_CountIf(D23:F23,"&gt;=3")</v>
       </c>
       <c r="B23" s="3" cm="1">
-        <f t="array" ref="B23">_xll.TBXLL_SqrtChecked(9)</f>
+        <f t="array" ref="B23">_xll.TBXLL_CountIf(D23:F23,"&gt;=3")</f>
+        <v>2</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
         <v>3</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="F23">
+        <v>4</v>
+      </c>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B24)</f>
-        <v>=TBXLL_TextOnly("25")</v>
-      </c>
-      <c r="B24" s="3" t="str" cm="1">
-        <f t="array" ref="B24">_xll.TBXLL_TextOnly("25")</f>
-        <v>OK: 25</v>
-      </c>
-      <c r="C24" s="6"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>=TBXLL_Now()</v>
+      </c>
+      <c r="B24" s="4" cm="1">
+        <f t="array" aca="1" ref="B24" ca="1">_xll.TBXLL_Now()</f>
+        <v>46082.320003935187</v>
+      </c>
+      <c r="C24" s="12"/>
       <c r="H24" s="7"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B25)</f>
-        <v>=TBXLL_Transpose({1;2;3})</v>
-      </c>
-      <c r="B25" s="3" cm="1">
-        <f t="array" ref="B25:D25">_xll.TBXLL_Transpose({1;2;3})</f>
-        <v>1</v>
-      </c>
-      <c r="C25" s="6">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
+        <f t="shared" ca="1" si="0"/>
+        <v>=NOW()</v>
+      </c>
+      <c r="B25" s="4">
+        <f ca="1">NOW()</f>
+        <v>46082.320003935187</v>
+      </c>
+      <c r="C25" s="6"/>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="str">
-        <f t="shared" ref="A26:A34" ca="1" si="2">_xlfn.FORMULATEXT(B26)</f>
-        <v>=TBXLL_Upper("mike")</v>
-      </c>
-      <c r="B26" s="3" t="str" cm="1">
-        <f t="array" ref="B26">_xll.TBXLL_Upper("mike")</f>
-        <v>MIKE</v>
+        <f ca="1">_xlfn.FORMULATEXT(B26)</f>
+        <v>=TBXLL_SqrtChecked(9)</v>
+      </c>
+      <c r="B26" s="3" cm="1">
+        <f t="array" ref="B26">_xll.TBXLL_SqrtChecked(9)</f>
+        <v>3</v>
       </c>
       <c r="C26" s="6"/>
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_RecalcCounter()</v>
-      </c>
-      <c r="B27" s="3" cm="1">
-        <f t="array" aca="1" ref="B27" ca="1">_xll.TBXLL_RecalcCounter()</f>
-        <v>2</v>
+        <f ca="1">_xlfn.FORMULATEXT(B27)</f>
+        <v>=TBXLL_TextOnly("25")</v>
+      </c>
+      <c r="B27" s="3" t="str" cm="1">
+        <f t="array" ref="B27">_xll.TBXLL_TextOnly("25")</f>
+        <v>OK: 25</v>
       </c>
       <c r="C27" s="6"/>
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_SumArray({1,2,3})</v>
+        <f ca="1">_xlfn.FORMULATEXT(B28)</f>
+        <v>=TBXLL_Transpose({1;2;3})</v>
       </c>
       <c r="B28" s="3" cm="1">
-        <f t="array" ref="B28">_xll.TBXLL_SumArray({1,2,3})</f>
-        <v>6</v>
-      </c>
-      <c r="C28" s="6"/>
+        <f t="array" ref="B28:D28">_xll.TBXLL_Transpose({1;2;3})</f>
+        <v>1</v>
+      </c>
+      <c r="C28" s="6">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_SumArray2({1,2,3})</v>
-      </c>
-      <c r="B29" s="3" cm="1">
-        <f t="array" ref="B29">_xll.TBXLL_SumArray2({1,2,3})</f>
-        <v>6</v>
+        <f t="shared" ref="A29:A37" ca="1" si="2">_xlfn.FORMULATEXT(B29)</f>
+        <v>=TBXLL_Upper("mike")</v>
+      </c>
+      <c r="B29" s="3" t="str" cm="1">
+        <f t="array" ref="B29">_xll.TBXLL_Upper("mike")</f>
+        <v>MIKE</v>
       </c>
       <c r="C29" s="6"/>
       <c r="H29" s="7"/>
@@ -944,53 +968,35 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>{=TBXLL_Join(D30:F31,TRUE)}</v>
-      </c>
-      <c r="B30" s="3" t="str">
-        <f t="array" ref="B30">_xll.TBXLL_Join(D30:F31,TRUE)</f>
-        <v>rc11,rc21,rc12,rc22,rc13,rc23</v>
+        <v>=TBXLL_RecalcCounter()</v>
+      </c>
+      <c r="B30" s="3" cm="1">
+        <f t="array" aca="1" ref="B30" ca="1">_xll.TBXLL_RecalcCounter()</f>
+        <v>8</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" t="s">
-        <v>2</v>
-      </c>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_Join(D30:F31,FALSE)</v>
-      </c>
-      <c r="B31" s="3" t="str" cm="1">
-        <f t="array" ref="B31">_xll.TBXLL_Join(D30:F31,FALSE)</f>
-        <v>rc11,rc12,rc13,rc21,rc22,rc23</v>
+        <v>=TBXLL_SumArray({1,2,3})</v>
+      </c>
+      <c r="B31" s="3" cm="1">
+        <f t="array" ref="B31">_xll.TBXLL_SumArray({1,2,3})</f>
+        <v>6</v>
       </c>
       <c r="C31" s="6"/>
-      <c r="D31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" t="s">
-        <v>5</v>
-      </c>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_Join({11,12,13;21,22,23},TRUE)</v>
-      </c>
-      <c r="B32" s="3" t="str" cm="1">
-        <f t="array" ref="B32">_xll.TBXLL_Join({11,12,13;21,22,23},TRUE)</f>
-        <v>11,21,12,22,13,23</v>
+        <v>=TBXLL_SumArray2({1,2,3})</v>
+      </c>
+      <c r="B32" s="3" cm="1">
+        <f t="array" ref="B32">_xll.TBXLL_SumArray2({1,2,3})</f>
+        <v>6</v>
       </c>
       <c r="C32" s="6"/>
       <c r="H32" s="7"/>
@@ -998,243 +1004,261 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_Join({11,12,13;21,22,23},FALSE)</v>
-      </c>
-      <c r="B33" s="3" t="str" cm="1">
-        <f t="array" ref="B33">_xll.TBXLL_Join({11,12,13;21,22,23},FALSE)</f>
-        <v>11,12,13,21,22,23</v>
+        <v>{=TBXLL_Join(D33:F34,TRUE)}</v>
+      </c>
+      <c r="B33" s="3" t="str">
+        <f t="array" ref="B33">_xll.TBXLL_Join(D33:F34,TRUE)</f>
+        <v>rc11,rc21,rc12,rc22,rc13,rc23</v>
       </c>
       <c r="C33" s="6"/>
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>2</v>
+      </c>
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=TBXLL_Join({11,12,13;21,22,23})</v>
+        <v>=TBXLL_Join(D33:F34,FALSE)</v>
       </c>
       <c r="B34" s="3" t="str" cm="1">
-        <f t="array" ref="B34">_xll.TBXLL_Join({11,12,13;21,22,23})</f>
-        <v>11,12,13,21,22,23</v>
+        <f t="array" ref="B34">_xll.TBXLL_Join(D33:F34,FALSE)</f>
+        <v>rc11,rc12,rc13,rc21,rc22,rc23</v>
       </c>
       <c r="C34" s="6"/>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="str">
-        <f t="shared" ref="A35:A45" ca="1" si="3">_xlfn.FORMULATEXT(B35)</f>
-        <v>=TBXLL_CellValue(testNamedRange)</v>
-      </c>
-      <c r="B35" s="3" t="b" cm="1">
-        <f t="array" ref="B35">_xll.TBXLL_CellValue(testNamedRange)</f>
-        <v>1</v>
-      </c>
-      <c r="C35" s="6" t="b">
-        <v>1</v>
-      </c>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_Join({11,12,13;21,22,23},TRUE)</v>
+      </c>
+      <c r="B35" s="3" t="str" cm="1">
+        <f t="array" ref="B35">_xll.TBXLL_Join({11,12,13;21,22,23},TRUE)</f>
+        <v>11,21,12,22,13,23</v>
+      </c>
+      <c r="C35" s="6"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_CellValue(C36)</v>
-      </c>
-      <c r="B36" s="3" cm="1">
-        <f t="array" ref="B36">_xll.TBXLL_CellValue(C36)</f>
-        <v>99</v>
-      </c>
-      <c r="C36" s="6">
-        <v>99</v>
-      </c>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_Join({11,12,13;21,22,23},FALSE)</v>
+      </c>
+      <c r="B36" s="3" t="str" cm="1">
+        <f t="array" ref="B36">_xll.TBXLL_Join({11,12,13;21,22,23},FALSE)</f>
+        <v>11,12,13,21,22,23</v>
+      </c>
+      <c r="C36" s="6"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_SheetName(D37)</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>=TBXLL_Join({11,12,13;21,22,23})</v>
       </c>
       <c r="B37" s="3" t="str" cm="1">
-        <f t="array" ref="B37">_xll.TBXLL_SheetName(D37)</f>
-        <v>[tests.xlsx]udf tests</v>
+        <f t="array" ref="B37">_xll.TBXLL_Join({11,12,13;21,22,23})</f>
+        <v>11,12,13,21,22,23</v>
       </c>
       <c r="C37" s="6"/>
       <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B38)</f>
-        <v>=TBXLL_CellAddress(C38)</v>
-      </c>
-      <c r="B38" s="13" t="str" cm="1">
-        <f t="array" ref="B38">_xll.TBXLL_CellAddress(C38)</f>
-        <v>$C$38</v>
-      </c>
-      <c r="C38" s="6"/>
+        <f t="shared" ref="A38:A48" ca="1" si="3">_xlfn.FORMULATEXT(B38)</f>
+        <v>=TBXLL_CellValue(testNamedRange)</v>
+      </c>
+      <c r="B38" s="3" t="b" cm="1">
+        <f t="array" ref="B38">_xll.TBXLL_CellValue(testNamedRange)</f>
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B39)</f>
-        <v>=TBXLL_CellAddress(Sheet2!C35)</v>
-      </c>
-      <c r="B39" s="13" t="str" cm="1">
-        <f t="array" ref="B39">_xll.TBXLL_CellAddress(Sheet2!C35)</f>
-        <v>$C$35</v>
-      </c>
-      <c r="C39" s="6"/>
+        <f t="shared" ca="1" si="3"/>
+        <v>=TBXLL_CellValue(C39)</v>
+      </c>
+      <c r="B39" s="3" cm="1">
+        <f t="array" ref="B39">_xll.TBXLL_CellValue(C39)</f>
+        <v>99</v>
+      </c>
+      <c r="C39" s="6">
+        <v>99</v>
+      </c>
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B40)</f>
-        <v>=TBXLL_CellAddress_Hidden(C38)</v>
-      </c>
-      <c r="B40" s="13" t="str" cm="1">
-        <f t="array" ref="B40">_xll.TBXLL_CellAddress_Hidden(C38)</f>
-        <v>$C$38</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>=TBXLL_SheetName(D40)</v>
+      </c>
+      <c r="B40" s="3" t="str" cm="1">
+        <f t="array" ref="B40">_xll.TBXLL_SheetName(D40)</f>
+        <v>[tests.xlsx]udf tests</v>
       </c>
       <c r="C40" s="6"/>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_IsEmptyCell(C41)</v>
-      </c>
-      <c r="B41" s="3" t="b" cm="1">
-        <f t="array" ref="B41">_xll.TBXLL_IsEmptyCell(C41)</f>
-        <v>1</v>
+        <f ca="1">_xlfn.FORMULATEXT(B41)</f>
+        <v>=TBXLL_CellAddress(C41)</v>
+      </c>
+      <c r="B41" s="13" t="str" cm="1">
+        <f t="array" ref="B41">_xll.TBXLL_CellAddress(C41)</f>
+        <v>$C$41</v>
       </c>
       <c r="C41" s="6"/>
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=TBXLL_TestMissing(3.6)</v>
-      </c>
-      <c r="B42" s="3" cm="1">
-        <f t="array" ref="B42">_xll.TBXLL_TestMissing(3.6)</f>
-        <v>4</v>
+        <f ca="1">_xlfn.FORMULATEXT(B42)</f>
+        <v>=TBXLL_CellAddress(Sheet2!C35)</v>
+      </c>
+      <c r="B42" s="13" t="str" cm="1">
+        <f t="array" ref="B42">_xll.TBXLL_CellAddress(Sheet2!C35)</f>
+        <v>$C$35</v>
       </c>
       <c r="C42" s="6"/>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>{=TBXLL_MultiplyArrays(D43:D45,E43:E45)}</v>
-      </c>
-      <c r="B43" s="3">
-        <f t="array" ref="B43:B45">_xll.TBXLL_MultiplyArrays(D43:D45,E43:E45)</f>
-        <v>2</v>
+        <f ca="1">_xlfn.FORMULATEXT(B43)</f>
+        <v>=TBXLL_CellAddress_Hidden(C41)</v>
+      </c>
+      <c r="B43" s="13" t="str" cm="1">
+        <f t="array" ref="B43">_xll.TBXLL_CellAddress_Hidden(C41)</f>
+        <v>$C$41</v>
       </c>
       <c r="C43" s="6"/>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>{=TBXLL_MultiplyArrays(D43:D45,E43:E45)}</v>
-      </c>
-      <c r="B44" s="3">
-        <v>20</v>
+        <v>=TBXLL_IsEmptyCell(C44)</v>
+      </c>
+      <c r="B44" s="3" t="b" cm="1">
+        <f t="array" ref="B44">_xll.TBXLL_IsEmptyCell(C44)</f>
+        <v>1</v>
       </c>
       <c r="C44" s="6"/>
-      <c r="D44">
-        <v>4</v>
-      </c>
-      <c r="E44">
-        <v>5</v>
-      </c>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>{=TBXLL_MultiplyArrays(D43:D45,E43:E45)}</v>
-      </c>
-      <c r="B45" s="3">
+        <v>=TBXLL_TestMissing(3.6)</v>
+      </c>
+      <c r="B45" s="3" cm="1">
+        <f t="array" ref="B45">_xll.TBXLL_TestMissing(3.6)</f>
         <v>4</v>
       </c>
       <c r="C45" s="6"/>
-      <c r="D45">
-        <v>2</v>
-      </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="str">
-        <f t="shared" ref="A46:A53" ca="1" si="4">_xlfn.FORMULATEXT(B46)</f>
-        <v>{=TBXLL_NormalizeArray({4,9,16,25})}</v>
-      </c>
-      <c r="B46" s="5">
-        <f t="array" ref="B46:E46">_xll.TBXLL_NormalizeArray({4,9,16,25})</f>
-        <v>7.407407407407407E-2</v>
-      </c>
-      <c r="C46" s="8">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D46" s="9">
-        <v>0.29629629629629628</v>
-      </c>
-      <c r="E46" s="9">
-        <v>0.46296296296296297</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>{=TBXLL_MultiplyArrays(D46:D48,E46:E48)}</v>
+      </c>
+      <c r="B46" s="3">
+        <f t="array" ref="B46:B48">_xll.TBXLL_MultiplyArrays(D46:D48,E46:E48)</f>
+        <v>2</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
       </c>
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=TBXLL_SpeedSafe(100)</v>
-      </c>
-      <c r="B47" s="3" cm="1">
-        <f t="array" ref="B47">_xll.TBXLL_SpeedSafe(100)</f>
-        <v>66671645.919710793</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>{=TBXLL_MultiplyArrays(D46:D48,E46:E48)}</v>
+      </c>
+      <c r="B47" s="3">
+        <v>20</v>
       </c>
       <c r="C47" s="6"/>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
       <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=TBXLL_SpeedUnsafe(100)</v>
-      </c>
-      <c r="B48" s="3" cm="1">
-        <f t="array" ref="B48">_xll.TBXLL_SpeedUnsafe(100)</f>
-        <v>66671645.919710793</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>{=TBXLL_MultiplyArrays(D46:D48,E46:E48)}</v>
+      </c>
+      <c r="B48" s="3">
+        <v>4</v>
       </c>
       <c r="C48" s="6"/>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="str">
-        <f t="shared" ref="A49" ca="1" si="5">_xlfn.FORMULATEXT(B49)</f>
-        <v>=TBXLL_Timestamp()</v>
-      </c>
-      <c r="B49" s="16" cm="1">
-        <f t="array" aca="1" ref="B49" ca="1">_xll.TBXLL_Timestamp()</f>
-        <v>249685.55196509999</v>
-      </c>
-      <c r="C49" s="6"/>
+        <f t="shared" ref="A49:A58" ca="1" si="4">_xlfn.FORMULATEXT(B49)</f>
+        <v>{=TBXLL_NormalizeArray({4,9,16,25})}</v>
+      </c>
+      <c r="B49" s="5">
+        <f t="array" ref="B49:E49">_xll.TBXLL_NormalizeArray({4,9,16,25})</f>
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="C49" s="8">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="E49" s="9">
+        <v>0.46296296296296297</v>
+      </c>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>=TBXLL_NumberName(9)</v>
-      </c>
-      <c r="B50" s="3" t="str" cm="1">
-        <f t="array" ref="B50">_xll.TBXLL_NumberName(9)</f>
-        <v>Nine</v>
+        <v>=TBXLL_SpeedSafe(100)</v>
+      </c>
+      <c r="B50" s="3" cm="1">
+        <f t="array" ref="B50">_xll.TBXLL_SpeedSafe(100)</f>
+        <v>66671645.919710793</v>
       </c>
       <c r="C50" s="6"/>
       <c r="H50" s="7"/>
@@ -1242,22 +1266,23 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>=TBXLL_RomanNumeral(9)</v>
-      </c>
-      <c r="B51" s="3" t="str" cm="1">
-        <f t="array" ref="B51">_xll.TBXLL_RomanNumeral(9)</f>
-        <v>IX</v>
-      </c>
+        <v>=TBXLL_SpeedUnsafe(100)</v>
+      </c>
+      <c r="B51" s="3" cm="1">
+        <f t="array" ref="B51">_xll.TBXLL_SpeedUnsafe(100)</f>
+        <v>66671645.919710793</v>
+      </c>
+      <c r="C51" s="6"/>
       <c r="H51" s="7"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>=TBXLL_AddDays(NOW(),7)</v>
-      </c>
-      <c r="B52" s="14" cm="1">
-        <f t="array" aca="1" ref="B52" ca="1">_xll.TBXLL_AddDays(NOW(),7)</f>
-        <v>46088.399229976851</v>
+        <f t="shared" ref="A52" ca="1" si="5">_xlfn.FORMULATEXT(B52)</f>
+        <v>=TBXLL_Timestamp()</v>
+      </c>
+      <c r="B52" s="16" cm="1">
+        <f t="array" aca="1" ref="B52" ca="1">_xll.TBXLL_Timestamp()</f>
+        <v>329241.8629525</v>
       </c>
       <c r="C52" s="6"/>
       <c r="H52" s="7"/>
@@ -1265,22 +1290,72 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3" t="str">
         <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_NumberName(9)</v>
+      </c>
+      <c r="B53" s="3" t="str" cm="1">
+        <f t="array" ref="B53">_xll.TBXLL_NumberName(9)</f>
+        <v>Nine</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_RomanNumeral(9)</v>
+      </c>
+      <c r="B54" s="3" t="str" cm="1">
+        <f t="array" ref="B54">_xll.TBXLL_RomanNumeral(9)</f>
+        <v>IX</v>
+      </c>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_AddDays(NOW(),7)</v>
+      </c>
+      <c r="B55" s="14" cm="1">
+        <f t="array" aca="1" ref="B55" ca="1">_xll.TBXLL_AddDays(NOW(),7)</f>
+        <v>46089.320003935187</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="3" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>=TBXLL_SumFP12(D46:E48)</v>
+      </c>
+      <c r="B56" cm="1">
+        <f t="array" ref="B56">_xll.TBXLL_SumFP12(D46:E48)</f>
+        <v>16</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="20" t="str">
+        <f t="shared" ca="1" si="4"/>
         <v>=TBXLL_FormatArray({1,2,3},"item")</v>
       </c>
-      <c r="B53" s="13" t="str" cm="1">
-        <f t="array" ref="B53:D53">_xll.TBXLL_FormatArray({1,2,3},"item")</f>
+      <c r="B57" s="13" t="str" cm="1">
+        <f t="array" ref="B57:D57">_xll.TBXLL_FormatArray({1,2,3},"item")</f>
         <v>item_1</v>
       </c>
-      <c r="C53" s="15" t="str">
+      <c r="C57" s="15" t="str">
         <v>item_2</v>
       </c>
-      <c r="D53" s="10" t="str">
+      <c r="D57" s="10" t="str">
         <v>item_3</v>
       </c>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="11"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="11"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>